<commit_message>
JM finished testing A+
</commit_message>
<xml_diff>
--- a/Aspen Plus Automation Transfer/Simulation Mapper - A+.xlsx
+++ b/Aspen Plus Automation Transfer/Simulation Mapper - A+.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836CF21A-D434-447B-8D5A-2AEBF4928F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30EC356-5EBF-445B-83D6-D5FC6DC3CA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pump &amp; Pump Curves" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2385" uniqueCount="1327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2387" uniqueCount="1329">
   <si>
     <r>
       <t>Capacity/Volumetirc flow rate (m</t>
@@ -2854,12 +2854,6 @@
     <t>5. Click on Mapper tab, in the Flowsheet Objects page. Click on object 'FEED' to enter the Object Mapping page.</t>
   </si>
   <si>
-    <t>MIX03</t>
-  </si>
-  <si>
-    <t>1. Launch ammonia.apwz file.</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Launch ICPEbegin-1.apwz file. </t>
   </si>
   <si>
@@ -3236,13 +3230,7 @@
     <t>Viscosity, mixture</t>
   </si>
   <si>
-    <t>4. Click on Mapper tab, in the Flowsheet Objects page. Click on object 'MIX03' to enter the Object Mapping page.</t>
-  </si>
-  <si>
     <t>5. Select 'Filter' for Map As column, select 'Create' for Workspace Object column.</t>
-  </si>
-  <si>
-    <t>9. Click on Explorer tab and expand the attributes of MIX03, check the attributes list below. The data in ABE should be in accordance with those in A+.</t>
   </si>
   <si>
     <t>MaterialPorts.MIX03-Inlet2.Flow.LiquidPhase.PvtProperties.Compressibility</t>
@@ -4168,7 +4156,25 @@
     <t>defect: CQ00770596 [SM] A+ - Column: "Feed Tray Number" is incorrect.</t>
   </si>
   <si>
-    <t>open file example Biodiesel Production from Vegetable Oil.bkp</t>
+    <t>Biodiesel Production from Vegetable Oil.bkp</t>
+  </si>
+  <si>
+    <t>MIXER1</t>
+  </si>
+  <si>
+    <t>1. Launch Biodiesel Production from Vegetable Oil.bkp file.</t>
+  </si>
+  <si>
+    <t>4. Click on Mapper tab, in the Flowsheet Objects page. Click on object 'MIXER1' to enter the Object Mapping page.</t>
+  </si>
+  <si>
+    <t>9. Click on Explorer tab and expand the attributes of MIXER1, check the attributes list below. The data in ABE should be in accordance with those in A+.</t>
+  </si>
+  <si>
+    <t>Properties are already added in template, so no need to add them</t>
+  </si>
+  <si>
+    <t>Go to Simulation-&gt; Streams -&gt; 2 -&gt; Results, select 'add properties', add  cloud point, freeze point, smoke point</t>
   </si>
 </sst>
 </file>
@@ -10787,7 +10793,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1">
       <c r="A1" s="96" t="s">
-        <v>1323</v>
+        <v>1319</v>
       </c>
       <c r="B1" s="93"/>
     </row>
@@ -11818,8 +11824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AA207"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11849,7 +11855,7 @@
         <v>885</v>
       </c>
       <c r="D3" s="114" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -11873,12 +11879,12 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -13244,16 +13250,19 @@
     </row>
     <row r="128" spans="1:6" ht="15.75">
       <c r="A128" s="176" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="B128" s="176" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="F128" s="111"/>
     </row>
     <row r="129" spans="1:27">
+      <c r="A129" t="s">
+        <v>1328</v>
+      </c>
       <c r="F129" s="41" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
     </row>
     <row r="130" spans="1:27">
@@ -13261,10 +13270,10 @@
         <v>10</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="D130" s="2">
         <v>201.88499999999999</v>
@@ -13275,10 +13284,10 @@
         <v>21</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="D131" s="3">
         <v>172.49700000000001</v>
@@ -13289,10 +13298,10 @@
         <v>45</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="D132" s="2">
         <v>27.370699999999999</v>
@@ -13369,8 +13378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C66" sqref="C65:C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13393,7 +13402,7 @@
         <v>65</v>
       </c>
       <c r="B3" s="86" t="s">
-        <v>1326</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75">
@@ -13401,7 +13410,7 @@
         <v>64</v>
       </c>
       <c r="B4" s="86" t="s">
-        <v>889</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75">
@@ -13411,7 +13420,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>890</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -13426,12 +13435,12 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>1016</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -13451,7 +13460,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>1018</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="16.5" thickBot="1">
@@ -13477,7 +13486,7 @@
       </c>
       <c r="G18" s="179"/>
       <c r="P18" s="8" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" thickBot="1">
@@ -13491,10 +13500,10 @@
         <v>4</v>
       </c>
       <c r="B20" s="187" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="C20" s="188" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="D20" s="186">
         <v>20255.5</v>
@@ -13536,7 +13545,7 @@
         <v>791</v>
       </c>
       <c r="C23" s="106" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="D23" s="29">
         <v>7.28E-3</v>
@@ -13547,7 +13556,7 @@
         <v>13</v>
       </c>
       <c r="B24" s="105" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="C24" s="105" t="s">
         <v>794</v>
@@ -13589,7 +13598,7 @@
         <v>17</v>
       </c>
       <c r="B27" s="105" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="C27" s="105" t="s">
         <v>800</v>
@@ -13617,7 +13626,7 @@
         <v>19</v>
       </c>
       <c r="B29" s="106" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="C29" s="106" t="s">
         <v>804</v>
@@ -13715,7 +13724,7 @@
         <v>30</v>
       </c>
       <c r="B36" s="105" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="C36" s="105" t="s">
         <v>818</v>
@@ -13785,10 +13794,10 @@
         <v>35</v>
       </c>
       <c r="B41" s="105" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="C41" s="105" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="D41" s="7">
         <v>3.5176150000000002</v>
@@ -13799,10 +13808,10 @@
         <v>36</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
       <c r="C42" s="105" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="D42" s="7">
         <v>73.224599999999995</v>
@@ -13869,10 +13878,10 @@
         <v>48</v>
       </c>
       <c r="B47" s="105" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="C47" s="105" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="D47" s="105">
         <v>0.18647</v>
@@ -13926,7 +13935,7 @@
         <v>58</v>
       </c>
       <c r="B51" s="105" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="C51" s="105" t="s">
         <v>848</v>
@@ -13935,7 +13944,7 @@
         <v>0.23039999999999999</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -13949,7 +13958,7 @@
         <v>850</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.75" thickBot="1">
@@ -13957,10 +13966,10 @@
         <v>60</v>
       </c>
       <c r="B53" s="217" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="C53" s="218" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="D53" s="145">
         <v>4535.08</v>
@@ -14046,117 +14055,120 @@
     </row>
     <row r="61" spans="1:6" ht="15.75">
       <c r="A61" s="180" t="s">
-        <v>1003</v>
+        <v>1001</v>
+      </c>
+      <c r="B61" s="64" t="s">
+        <v>1327</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
     </row>
   </sheetData>
@@ -14190,7 +14202,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1">
       <c r="A1" s="96" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="B1" s="93"/>
       <c r="G1" s="124"/>
@@ -14198,7 +14210,7 @@
     <row r="2" spans="1:10" ht="15.75" thickTop="1"/>
     <row r="3" spans="1:10" ht="15.75">
       <c r="A3" s="125" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75">
@@ -14211,7 +14223,7 @@
         <v>65</v>
       </c>
       <c r="B5" s="123" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -14224,10 +14236,10 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="123" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="B7" s="123" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="16.5" thickBot="1">
@@ -14255,7 +14267,7 @@
         <v>191</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>1322</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1">
@@ -14267,89 +14279,89 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="191" t="s">
+        <v>905</v>
+      </c>
+      <c r="B12" s="153" t="s">
+        <v>906</v>
+      </c>
+      <c r="C12" s="153" t="s">
+        <v>906</v>
+      </c>
+      <c r="D12" s="153" t="s">
         <v>907</v>
-      </c>
-      <c r="B12" s="153" t="s">
-        <v>908</v>
-      </c>
-      <c r="C12" s="153" t="s">
-        <v>908</v>
-      </c>
-      <c r="D12" s="153" t="s">
-        <v>909</v>
       </c>
       <c r="E12" s="153"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="118" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="D13" s="6">
         <v>17.898499999999999</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="J13" s="119"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="118" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="D14" s="6">
         <v>17.898499999999999</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="118" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="D15" s="6">
         <v>1.3423799999999999</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1">
       <c r="A16" s="120" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="B16" s="121" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="C16" s="121" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="D16" s="121" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E16" s="121"/>
     </row>
     <row r="20" spans="1:7" ht="15.75">
       <c r="A20" s="125" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75">
@@ -14362,7 +14374,7 @@
         <v>65</v>
       </c>
       <c r="B22" s="123" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -14375,10 +14387,10 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="123" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="B24" s="123" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16.5" thickBot="1">
@@ -14406,7 +14418,7 @@
         <v>191</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1">
@@ -14418,88 +14430,88 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="191" t="s">
+        <v>905</v>
+      </c>
+      <c r="B29" s="153" t="s">
+        <v>906</v>
+      </c>
+      <c r="C29" s="153" t="s">
+        <v>906</v>
+      </c>
+      <c r="D29" s="153" t="s">
         <v>907</v>
-      </c>
-      <c r="B29" s="153" t="s">
-        <v>908</v>
-      </c>
-      <c r="C29" s="153" t="s">
-        <v>908</v>
-      </c>
-      <c r="D29" s="153" t="s">
-        <v>909</v>
       </c>
       <c r="E29" s="153"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="118" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="D30" s="6">
         <v>3134.49</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="118" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="D31" s="6">
         <v>5545.72</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="118" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="D32" s="6">
         <v>24.825099999999999</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1">
       <c r="A33" s="120" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="B33" s="121" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="C33" s="121" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="D33" s="121" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E33" s="121"/>
     </row>
     <row r="37" spans="1:7" ht="15.75">
       <c r="A37" s="125" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75">
@@ -14512,7 +14524,7 @@
         <v>65</v>
       </c>
       <c r="B39" s="123" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -14520,15 +14532,15 @@
         <v>64</v>
       </c>
       <c r="B40" s="123" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="123" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="B41" s="123" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="16.5" thickBot="1">
@@ -14556,7 +14568,7 @@
         <v>191</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" thickBot="1">
@@ -14568,90 +14580,90 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="118" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="118" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="D47" s="6">
         <v>128.375</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="118" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="D48" s="6">
         <v>128.375</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="118" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="D49" s="6">
         <v>9.94909</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" thickBot="1">
       <c r="A50" s="120" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="B50" s="121" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="C50" s="121" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="D50" s="121">
         <v>44.533799999999999</v>
       </c>
       <c r="E50" s="121" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75">
       <c r="A54" s="125" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.75">
@@ -14664,10 +14676,10 @@
         <v>65</v>
       </c>
       <c r="B56" s="123" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="C56" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -14680,10 +14692,10 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="123" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="B58" s="123" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="16.5" thickBot="1">
@@ -14711,7 +14723,7 @@
         <v>191</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1" thickBot="1">
@@ -14723,41 +14735,41 @@
     </row>
     <row r="63" spans="1:7" ht="15.75" customHeight="1">
       <c r="A63" s="118" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D63" s="6">
         <v>69.946700000000007</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="118" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="D64" s="6">
         <v>5.4208699999999999</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15.75">
       <c r="A68" s="125" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15.75">
@@ -14770,7 +14782,7 @@
         <v>65</v>
       </c>
       <c r="B70" s="123" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -14783,10 +14795,10 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="123" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="B72" s="123" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="16.5" thickBot="1">
@@ -14814,7 +14826,7 @@
         <v>191</v>
       </c>
       <c r="G75" s="8" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="15.75" thickBot="1">
@@ -14826,90 +14838,90 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="118" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="E77" s="6"/>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="118" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="D78" s="44">
         <v>935.5</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="118" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="D79" s="6">
         <v>1655.14</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="118" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="D80" s="6">
         <v>7.40916</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="15.75" thickBot="1">
       <c r="A81" s="121" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="B81" s="121" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="C81" s="121" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="D81" s="121">
         <v>221.44300000000001</v>
       </c>
       <c r="E81" s="121" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="15.75">
       <c r="A85" s="125" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="15.75">
@@ -14922,7 +14934,7 @@
         <v>65</v>
       </c>
       <c r="B87" s="123" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -14930,12 +14942,12 @@
         <v>64</v>
       </c>
       <c r="B88" s="123" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -14950,62 +14962,62 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="97" spans="1:14">
       <c r="A97" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
     </row>
     <row r="98" spans="1:14">
       <c r="A98" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
     </row>
     <row r="99" spans="1:14">
       <c r="A99" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
     </row>
     <row r="100" spans="1:14">
       <c r="A100" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="101" spans="1:14">
       <c r="A101" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
     </row>
     <row r="102" spans="1:14">
       <c r="A102" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="103" spans="1:14">
       <c r="A103" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="104" spans="1:14">
       <c r="A104" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="106" spans="1:14" ht="16.5" thickBot="1">
@@ -15033,10 +15045,10 @@
         <v>191</v>
       </c>
       <c r="G107" s="8" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="N107" s="8" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
     </row>
     <row r="108" spans="1:14" ht="16.5" customHeight="1" thickBot="1">
@@ -15048,173 +15060,173 @@
     </row>
     <row r="109" spans="1:14">
       <c r="A109" s="6" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="E109" s="6"/>
     </row>
     <row r="110" spans="1:14">
       <c r="A110" s="6" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="D110" s="6">
         <v>-32.410800000000002</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
     </row>
     <row r="111" spans="1:14">
       <c r="A111" s="6" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="D111" s="6">
         <v>87008.8</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="6" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="D112" s="6">
         <v>0.3902041</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="6" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="D113" s="6">
         <v>6.5211699999999997</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="6" t="s">
+        <v>950</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>951</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>951</v>
+      </c>
+      <c r="D114" s="6" t="s">
         <v>952</v>
-      </c>
-      <c r="B114" s="6" t="s">
-        <v>953</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>953</v>
-      </c>
-      <c r="D114" s="6" t="s">
-        <v>954</v>
       </c>
       <c r="E114" s="6"/>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="6" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="D115" s="6">
         <v>412.96100000000001</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="6" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="D116" s="6">
         <v>864.67700000000002</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="6" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="D117" s="6">
         <v>3.71665</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="6" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="D118" s="6">
         <v>97.752099999999999</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="15.75">
       <c r="A125" s="125" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="15.75">
@@ -15227,7 +15239,7 @@
         <v>65</v>
       </c>
       <c r="B127" s="123" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -15240,10 +15252,10 @@
     </row>
     <row r="129" spans="1:7">
       <c r="A129" s="123" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="B129" s="123" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="16.5" thickBot="1">
@@ -15271,7 +15283,7 @@
         <v>191</v>
       </c>
       <c r="G132" s="8" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="15.75" customHeight="1" thickBot="1">
@@ -15283,28 +15295,28 @@
     </row>
     <row r="134" spans="1:7">
       <c r="A134" s="118" t="s">
+        <v>905</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>906</v>
+      </c>
+      <c r="C134" s="6" t="s">
+        <v>906</v>
+      </c>
+      <c r="D134" s="6" t="s">
         <v>907</v>
-      </c>
-      <c r="B134" s="6" t="s">
-        <v>908</v>
-      </c>
-      <c r="C134" s="6" t="s">
-        <v>908</v>
-      </c>
-      <c r="D134" s="6" t="s">
-        <v>909</v>
       </c>
       <c r="E134" s="6"/>
     </row>
     <row r="135" spans="1:7">
       <c r="A135" s="118" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="D135" s="6">
         <v>-34855.000403600003</v>
@@ -15315,13 +15327,13 @@
     </row>
     <row r="136" spans="1:7">
       <c r="A136" s="118" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="D136" s="6">
         <v>34855.004999999997</v>
@@ -15332,36 +15344,36 @@
     </row>
     <row r="137" spans="1:7">
       <c r="A137" s="118" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="D137" s="6">
         <v>0.78423799999999999</v>
       </c>
       <c r="E137" s="6" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="15.75" thickBot="1">
       <c r="A138" s="120" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="B138" s="121" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="C138" s="121" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="D138" s="121" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E138" s="121" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
     </row>
   </sheetData>
@@ -15431,7 +15443,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1">
       <c r="A1" s="96" t="s">
-        <v>1306</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1"/>
@@ -15440,10 +15452,10 @@
         <v>65</v>
       </c>
       <c r="B3" s="86" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="D3" t="s">
-        <v>1298</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75">
@@ -15451,10 +15463,10 @@
         <v>64</v>
       </c>
       <c r="B4" s="86" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
       <c r="D4" t="s">
-        <v>1325</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75">
@@ -15464,7 +15476,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -15479,42 +15491,42 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>1299</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>1307</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>1318</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>1308</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="16.5" thickBot="1">
       <c r="A17" t="s">
-        <v>1317</v>
+        <v>1313</v>
       </c>
       <c r="I17" s="96" t="s">
         <v>550</v>
@@ -15522,32 +15534,32 @@
     </row>
     <row r="18" spans="1:12" ht="15.75" thickTop="1">
       <c r="A18" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="117" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>1309</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>1310</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15.75">
       <c r="A23" s="86" t="s">
-        <v>1300</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15.75" thickBot="1">
       <c r="A24" s="8" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
@@ -15558,13 +15570,13 @@
         <v>37</v>
       </c>
       <c r="C25" s="233" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="D25" s="232" t="s">
-        <v>1031</v>
+        <v>1027</v>
       </c>
       <c r="E25" s="232" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
       <c r="F25" s="234" t="s">
         <v>191</v>
@@ -15575,13 +15587,13 @@
         <v>1</v>
       </c>
       <c r="B26" s="220" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
       <c r="C26" s="135" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="D26" s="135" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="E26" s="193">
         <v>7</v>
@@ -15593,13 +15605,13 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>1035</v>
+        <v>1031</v>
       </c>
       <c r="C27" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="D27" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
       <c r="E27" s="197">
         <v>7</v>
@@ -15611,13 +15623,13 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="C28" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
       <c r="D28" t="s">
-        <v>1040</v>
+        <v>1036</v>
       </c>
       <c r="E28" s="197">
         <v>100000</v>
@@ -15631,13 +15643,13 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>1041</v>
+        <v>1037</v>
       </c>
       <c r="C29" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
       <c r="D29" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
       <c r="E29" s="197">
         <v>200833</v>
@@ -15651,13 +15663,13 @@
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>1044</v>
+        <v>1040</v>
       </c>
       <c r="C30" t="s">
-        <v>1045</v>
+        <v>1041</v>
       </c>
       <c r="D30" t="s">
-        <v>1045</v>
+        <v>1041</v>
       </c>
       <c r="E30" s="197">
         <v>8105.9900781595397</v>
@@ -15671,13 +15683,13 @@
         <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>1046</v>
+        <v>1042</v>
       </c>
       <c r="C31" t="s">
-        <v>1047</v>
+        <v>1043</v>
       </c>
       <c r="D31" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
       <c r="E31" s="197">
         <v>2</v>
@@ -15689,13 +15701,13 @@
         <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
       <c r="C32" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
       <c r="D32" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
       <c r="E32" s="197">
         <v>6.2373165299999998E-2</v>
@@ -15708,13 +15720,13 @@
         <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
       <c r="C33" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
       <c r="D33" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
       <c r="E33" s="199">
         <v>-38920792</v>
@@ -15728,13 +15740,13 @@
         <v>76</v>
       </c>
       <c r="B34" t="s">
-        <v>1051</v>
+        <v>1047</v>
       </c>
       <c r="C34" t="s">
-        <v>1052</v>
+        <v>1048</v>
       </c>
       <c r="D34" t="s">
-        <v>1053</v>
+        <v>1049</v>
       </c>
       <c r="E34" s="197">
         <v>338.06271900000002</v>
@@ -15748,13 +15760,13 @@
         <v>61</v>
       </c>
       <c r="B35" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
       <c r="C35" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
       <c r="D35" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
       <c r="E35" s="199">
         <v>2326000</v>
@@ -15768,13 +15780,13 @@
         <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>1055</v>
+        <v>1051</v>
       </c>
       <c r="C36" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
       <c r="D36" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
       <c r="E36" s="197">
         <v>573.20999700000004</v>
@@ -15786,19 +15798,19 @@
         <v>77</v>
       </c>
       <c r="B37" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
       <c r="C37" t="s">
-        <v>1058</v>
+        <v>1054</v>
       </c>
       <c r="D37" t="s">
-        <v>1058</v>
+        <v>1054</v>
       </c>
       <c r="E37" s="199">
         <v>1.5836709900000001E-3</v>
       </c>
       <c r="F37" s="206" t="s">
-        <v>1059</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="38" spans="1:16">
@@ -15806,19 +15818,19 @@
         <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>1060</v>
+        <v>1056</v>
       </c>
       <c r="C38" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
       <c r="D38" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="E38" s="197">
         <v>0.92051691800000002</v>
       </c>
       <c r="F38" s="206" t="s">
-        <v>1059</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" thickBot="1">
@@ -15826,13 +15838,13 @@
         <v>79</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>1064</v>
+        <v>1060</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>1064</v>
+        <v>1060</v>
       </c>
       <c r="E39" s="201">
         <v>397.86855100000002</v>
@@ -15863,15 +15875,15 @@
     </row>
     <row r="44" spans="1:16">
       <c r="I44" s="8" t="s">
-        <v>1302</v>
+        <v>1298</v>
       </c>
       <c r="P44" s="8" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="15.75" thickBot="1">
       <c r="A45" s="8" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="46" spans="1:16">
@@ -15879,10 +15891,10 @@
         <v>6</v>
       </c>
       <c r="B46" s="135" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="C46" s="135" t="s">
-        <v>1067</v>
+        <v>1063</v>
       </c>
       <c r="D46" s="135"/>
       <c r="E46" s="193">
@@ -15890,7 +15902,7 @@
       </c>
       <c r="F46" s="205"/>
       <c r="G46" s="8" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
       <c r="H46" s="8"/>
     </row>
@@ -15899,13 +15911,13 @@
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>1068</v>
+        <v>1064</v>
       </c>
       <c r="C47" t="s">
-        <v>1069</v>
+        <v>1065</v>
       </c>
       <c r="D47" t="s">
-        <v>1070</v>
+        <v>1066</v>
       </c>
       <c r="E47" s="197">
         <v>5</v>
@@ -15917,19 +15929,19 @@
         <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>1072</v>
+        <v>1068</v>
       </c>
       <c r="C48" t="s">
-        <v>1073</v>
+        <v>1069</v>
       </c>
       <c r="D48" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
       <c r="E48" s="197">
         <v>3.2004000000000001</v>
       </c>
       <c r="F48" s="206" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -15937,19 +15949,19 @@
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
       <c r="C49" t="s">
-        <v>1077</v>
+        <v>1073</v>
       </c>
       <c r="D49" t="s">
-        <v>1078</v>
+        <v>1074</v>
       </c>
       <c r="E49" s="197">
         <v>1.2</v>
       </c>
       <c r="F49" s="206" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -15957,16 +15969,16 @@
         <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>1079</v>
+        <v>1075</v>
       </c>
       <c r="C50" t="s">
-        <v>1080</v>
+        <v>1076</v>
       </c>
       <c r="D50" t="s">
-        <v>1081</v>
+        <v>1077</v>
       </c>
       <c r="E50" s="197" t="s">
-        <v>1082</v>
+        <v>1078</v>
       </c>
       <c r="F50" s="206"/>
       <c r="G50" s="209"/>
@@ -15976,16 +15988,16 @@
         <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
       <c r="C51" t="s">
-        <v>1084</v>
+        <v>1080</v>
       </c>
       <c r="D51" t="s">
-        <v>1085</v>
+        <v>1081</v>
       </c>
       <c r="E51" s="197" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
       <c r="F51" s="206"/>
       <c r="J51" s="81"/>
@@ -15995,19 +16007,19 @@
         <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>1087</v>
+        <v>1083</v>
       </c>
       <c r="C52" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
       <c r="D52" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
       <c r="E52" s="197">
         <v>130</v>
       </c>
       <c r="F52" s="206" t="s">
-        <v>1089</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="15.75" thickBot="1">
@@ -16015,13 +16027,13 @@
         <v>56</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>1093</v>
+        <v>1089</v>
       </c>
       <c r="E53" s="203">
         <v>391.01516410289099</v>
@@ -16035,22 +16047,22 @@
         <v>23</v>
       </c>
       <c r="B54" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
       <c r="C54" s="135" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="D54" s="135" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
       <c r="E54" s="193">
         <v>0.88390000000000002</v>
       </c>
       <c r="F54" s="205" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
       <c r="H54" s="8"/>
     </row>
@@ -16059,13 +16071,13 @@
         <v>24</v>
       </c>
       <c r="B55" t="s">
-        <v>1097</v>
+        <v>1093</v>
       </c>
       <c r="C55" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
       <c r="D55" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
       <c r="E55" s="197">
         <v>1</v>
@@ -16077,19 +16089,19 @@
         <v>25</v>
       </c>
       <c r="B56" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
       <c r="C56" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
       <c r="D56" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="E56" s="197">
         <v>0.76200000000000001</v>
       </c>
       <c r="F56" s="206" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -16097,19 +16109,19 @@
         <v>26</v>
       </c>
       <c r="B57" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="C57" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="D57" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
       <c r="E57" s="197">
         <v>0.61361525663460903</v>
       </c>
       <c r="F57" s="206" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -16117,19 +16129,19 @@
         <v>27</v>
       </c>
       <c r="B58" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
       <c r="C58" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="D58" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="E58" s="197">
         <v>0.33744501407333399</v>
       </c>
       <c r="F58" s="206" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -16137,13 +16149,13 @@
         <v>28</v>
       </c>
       <c r="B59" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
       <c r="C59" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
       <c r="D59" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="E59" s="197">
         <v>0.1</v>
@@ -16155,19 +16167,19 @@
         <v>29</v>
       </c>
       <c r="B60" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="C60" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="D60" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="E60" s="197">
         <v>244.2596455</v>
       </c>
       <c r="F60" s="206" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -16175,19 +16187,19 @@
         <v>30</v>
       </c>
       <c r="B61" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
       <c r="C61" t="s">
-        <v>1115</v>
+        <v>1111</v>
       </c>
       <c r="D61" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
       <c r="E61" s="197">
         <v>244.2596455</v>
       </c>
       <c r="F61" s="206" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -16195,19 +16207,19 @@
         <v>31</v>
       </c>
       <c r="B62" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
       <c r="C62" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
       <c r="D62" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
       <c r="E62" s="197">
         <v>0.13808512128063699</v>
       </c>
       <c r="F62" s="206" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -16215,19 +16227,19 @@
         <v>32</v>
       </c>
       <c r="B63" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
       <c r="C63" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
       <c r="D63" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
       <c r="E63" s="197">
         <v>0.13808512128063699</v>
       </c>
       <c r="F63" s="206" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="15.75" thickBot="1">
@@ -16235,19 +16247,19 @@
         <v>33</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>1125</v>
+        <v>1121</v>
       </c>
       <c r="E64" s="203">
         <v>0.79053988194818903</v>
       </c>
       <c r="F64" s="207" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -16255,22 +16267,22 @@
         <v>69</v>
       </c>
       <c r="B65" s="135" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
       <c r="C65" s="135" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
       <c r="D65" s="135" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
       <c r="E65" s="193">
         <v>6.9793052799286895E-2</v>
       </c>
       <c r="F65" s="205" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
       <c r="H65" s="8"/>
     </row>
@@ -16279,19 +16291,19 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="C66" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="D66" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="E66" s="197">
         <v>64.401512049797702</v>
       </c>
       <c r="F66" s="206" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -16299,13 +16311,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>1130</v>
+        <v>1126</v>
       </c>
       <c r="C67" t="s">
-        <v>1130</v>
+        <v>1126</v>
       </c>
       <c r="D67" t="s">
-        <v>1130</v>
+        <v>1126</v>
       </c>
       <c r="E67" s="197">
         <v>1.00589</v>
@@ -16317,13 +16329,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="C68" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="D68" t="s">
-        <v>1132</v>
+        <v>1128</v>
       </c>
       <c r="E68" s="197">
         <v>1.1140699999999999</v>
@@ -16335,13 +16347,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
       <c r="C69" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
       <c r="D69" t="s">
-        <v>1134</v>
+        <v>1130</v>
       </c>
       <c r="E69" s="197">
         <v>2.9825200000000001</v>
@@ -16353,13 +16365,13 @@
         <v>64</v>
       </c>
       <c r="B70" s="20" t="s">
-        <v>1135</v>
+        <v>1131</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>1136</v>
+        <v>1132</v>
       </c>
       <c r="D70" s="20" t="s">
-        <v>1136</v>
+        <v>1132</v>
       </c>
       <c r="E70" s="203">
         <v>0.95</v>
@@ -16368,7 +16380,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="I72" s="8" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -16376,7 +16388,7 @@
     </row>
     <row r="77" spans="1:9" ht="15.75" thickBot="1">
       <c r="A77" s="8" t="s">
-        <v>1137</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -16384,20 +16396,20 @@
         <v>9</v>
       </c>
       <c r="B78" s="135" t="s">
-        <v>1138</v>
+        <v>1134</v>
       </c>
       <c r="C78" s="135" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
       <c r="D78" s="135" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="E78" s="193">
         <v>7</v>
       </c>
       <c r="F78" s="205"/>
       <c r="G78" s="8" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
       <c r="H78" s="8"/>
     </row>
@@ -16406,13 +16418,13 @@
         <v>10</v>
       </c>
       <c r="B79" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
       <c r="C79" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="D79" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
       <c r="E79" s="197">
         <v>394.14797900000002</v>
@@ -16426,13 +16438,13 @@
         <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="C80" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="D80" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
       <c r="E80" s="197">
         <v>200833</v>
@@ -16446,19 +16458,19 @@
         <v>12</v>
       </c>
       <c r="B81" t="s">
-        <v>1147</v>
+        <v>1143</v>
       </c>
       <c r="C81" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="D81" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="E81" s="197">
         <v>0.91014285399999995</v>
       </c>
       <c r="F81" s="206" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -16466,13 +16478,13 @@
         <v>13</v>
       </c>
       <c r="B82" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="C82" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
       <c r="D82" t="s">
-        <v>1153</v>
+        <v>1149</v>
       </c>
       <c r="E82" s="197">
         <v>0.79751498600000004</v>
@@ -16486,19 +16498,19 @@
         <v>14</v>
       </c>
       <c r="B83" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="C83" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
       <c r="D83" t="s">
-        <v>1156</v>
+        <v>1152</v>
       </c>
       <c r="E83" s="197">
         <v>18.014480599999999</v>
       </c>
       <c r="F83" s="206" t="s">
-        <v>1157</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -16506,19 +16518,19 @@
         <v>15</v>
       </c>
       <c r="B84" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
       <c r="C84" t="s">
-        <v>1159</v>
+        <v>1155</v>
       </c>
       <c r="D84" t="s">
-        <v>1160</v>
+        <v>1156</v>
       </c>
       <c r="E84" s="197">
         <v>1.1412235100000001</v>
       </c>
       <c r="F84" s="206" t="s">
-        <v>1161</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -16526,13 +16538,13 @@
         <v>16</v>
       </c>
       <c r="B85" t="s">
-        <v>1162</v>
+        <v>1158</v>
       </c>
       <c r="C85" t="s">
-        <v>1163</v>
+        <v>1159</v>
       </c>
       <c r="D85" t="s">
-        <v>1164</v>
+        <v>1160</v>
       </c>
       <c r="E85" s="197">
         <v>393.49675000000002</v>
@@ -16546,13 +16558,13 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>1165</v>
+        <v>1161</v>
       </c>
       <c r="C86" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="D86" t="s">
-        <v>1167</v>
+        <v>1163</v>
       </c>
       <c r="E86" s="197">
         <v>1.8562601799999998E-2</v>
@@ -16566,19 +16578,19 @@
         <v>18</v>
       </c>
       <c r="B87" t="s">
-        <v>1168</v>
+        <v>1164</v>
       </c>
       <c r="C87" t="s">
-        <v>1169</v>
+        <v>1165</v>
       </c>
       <c r="D87" t="s">
-        <v>1170</v>
+        <v>1166</v>
       </c>
       <c r="E87" s="197">
         <v>17.4934762</v>
       </c>
       <c r="F87" s="206" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -16586,19 +16598,19 @@
         <v>19</v>
       </c>
       <c r="B88" t="s">
-        <v>1171</v>
+        <v>1167</v>
       </c>
       <c r="C88" t="s">
-        <v>1172</v>
+        <v>1168</v>
       </c>
       <c r="D88" t="s">
-        <v>1173</v>
+        <v>1169</v>
       </c>
       <c r="E88" s="197">
         <v>2.2796017399999999E-4</v>
       </c>
       <c r="F88" s="206" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="15.75" thickBot="1">
@@ -16606,19 +16618,19 @@
         <v>20</v>
       </c>
       <c r="B89" s="215" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>1176</v>
+        <v>1172</v>
       </c>
       <c r="D89" s="204" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="E89" s="203">
         <v>942.40432099999998</v>
       </c>
       <c r="F89" s="207" t="s">
-        <v>1161</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -16651,7 +16663,7 @@
     <row r="99" spans="1:9">
       <c r="A99" s="212"/>
       <c r="I99" s="8" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="24" customHeight="1">
@@ -16659,7 +16671,7 @@
     </row>
     <row r="101" spans="1:9" ht="15.75" thickBot="1">
       <c r="A101" s="8" t="s">
-        <v>1185</v>
+        <v>1181</v>
       </c>
       <c r="C101" s="20"/>
       <c r="D101" s="20"/>
@@ -16671,18 +16683,18 @@
         <v>34</v>
       </c>
       <c r="B102" s="213" t="s">
-        <v>1182</v>
+        <v>1178</v>
       </c>
       <c r="C102" s="135" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="D102" s="135"/>
       <c r="E102" s="213" t="s">
-        <v>1184</v>
+        <v>1180</v>
       </c>
       <c r="F102" s="195"/>
       <c r="G102" s="8" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
       <c r="H102" s="8"/>
     </row>
@@ -16691,13 +16703,13 @@
         <v>36</v>
       </c>
       <c r="B103" s="209" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
       <c r="C103" t="s">
-        <v>1187</v>
+        <v>1183</v>
       </c>
       <c r="D103" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="E103" s="197">
         <v>397.86200000000002</v>
@@ -16711,13 +16723,13 @@
         <v>37</v>
       </c>
       <c r="B104" s="209" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="C104" t="s">
-        <v>1190</v>
+        <v>1186</v>
       </c>
       <c r="D104" t="s">
-        <v>1191</v>
+        <v>1187</v>
       </c>
       <c r="E104" s="197">
         <v>196667</v>
@@ -16731,19 +16743,19 @@
         <v>38</v>
       </c>
       <c r="B105" s="209" t="s">
-        <v>1192</v>
+        <v>1188</v>
       </c>
       <c r="C105" t="s">
-        <v>1193</v>
+        <v>1189</v>
       </c>
       <c r="D105" t="s">
-        <v>1194</v>
+        <v>1190</v>
       </c>
       <c r="E105" s="197">
         <v>18.0152</v>
       </c>
       <c r="F105" s="206" t="s">
-        <v>1157</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -16751,19 +16763,19 @@
         <v>39</v>
       </c>
       <c r="B106" s="209" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="C106" t="s">
-        <v>1196</v>
+        <v>1192</v>
       </c>
       <c r="D106" t="s">
-        <v>1197</v>
+        <v>1193</v>
       </c>
       <c r="E106" s="197">
         <v>1.08371</v>
       </c>
       <c r="F106" s="206" t="s">
-        <v>1161</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -16771,19 +16783,19 @@
         <v>40</v>
       </c>
       <c r="B107" s="209" t="s">
-        <v>1198</v>
+        <v>1194</v>
       </c>
       <c r="C107" t="s">
-        <v>1199</v>
+        <v>1195</v>
       </c>
       <c r="D107" t="s">
-        <v>1200</v>
+        <v>1196</v>
       </c>
       <c r="E107" s="199">
         <v>1.35079E-5</v>
       </c>
       <c r="F107" s="206" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -16791,19 +16803,19 @@
         <v>41</v>
       </c>
       <c r="B108" s="209" t="s">
-        <v>1201</v>
+        <v>1197</v>
       </c>
       <c r="C108" t="s">
-        <v>1202</v>
+        <v>1198</v>
       </c>
       <c r="D108" t="s">
-        <v>1203</v>
+        <v>1199</v>
       </c>
       <c r="E108" s="197">
         <v>17.499500000000001</v>
       </c>
       <c r="F108" s="206" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -16811,13 +16823,13 @@
         <v>42</v>
       </c>
       <c r="B109" s="209" t="s">
-        <v>1204</v>
+        <v>1200</v>
       </c>
       <c r="C109" t="s">
-        <v>1205</v>
+        <v>1201</v>
       </c>
       <c r="D109" t="s">
-        <v>1206</v>
+        <v>1202</v>
       </c>
       <c r="E109" s="197">
         <v>16.1477</v>
@@ -16831,13 +16843,13 @@
         <v>43</v>
       </c>
       <c r="B110" s="209" t="s">
-        <v>1207</v>
+        <v>1203</v>
       </c>
       <c r="C110" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="D110" t="s">
-        <v>1209</v>
+        <v>1205</v>
       </c>
       <c r="E110" s="197">
         <v>338.06299999999999</v>
@@ -16851,13 +16863,13 @@
         <v>44</v>
       </c>
       <c r="B111" s="209" t="s">
-        <v>1210</v>
+        <v>1206</v>
       </c>
       <c r="C111" t="s">
-        <v>1211</v>
+        <v>1207</v>
       </c>
       <c r="D111" t="s">
-        <v>1212</v>
+        <v>1208</v>
       </c>
       <c r="E111" s="214">
         <v>100000</v>
@@ -16871,19 +16883,19 @@
         <v>45</v>
       </c>
       <c r="B112" s="209" t="s">
-        <v>1213</v>
+        <v>1209</v>
       </c>
       <c r="C112" t="s">
-        <v>1214</v>
+        <v>1210</v>
       </c>
       <c r="D112" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="E112" s="197">
         <v>18.0852</v>
       </c>
       <c r="F112" s="206" t="s">
-        <v>1157</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="113" spans="1:9">
@@ -16891,19 +16903,19 @@
         <v>46</v>
       </c>
       <c r="B113" s="209" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="C113" t="s">
-        <v>1217</v>
+        <v>1213</v>
       </c>
       <c r="D113" t="s">
-        <v>1218</v>
+        <v>1214</v>
       </c>
       <c r="E113" s="197">
         <v>868.65300000000002</v>
       </c>
       <c r="F113" s="206" t="s">
-        <v>1161</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="114" spans="1:9">
@@ -16911,19 +16923,19 @@
         <v>47</v>
       </c>
       <c r="B114" s="209" t="s">
-        <v>1219</v>
+        <v>1215</v>
       </c>
       <c r="C114" t="s">
-        <v>1220</v>
+        <v>1216</v>
       </c>
       <c r="D114" t="s">
-        <v>1221</v>
+        <v>1217</v>
       </c>
       <c r="E114" s="14">
         <v>3.7827716000000001E-4</v>
       </c>
       <c r="F114" s="206" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="115" spans="1:9">
@@ -16931,19 +16943,19 @@
         <v>48</v>
       </c>
       <c r="B115" s="209" t="s">
-        <v>1222</v>
+        <v>1218</v>
       </c>
       <c r="C115" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="D115" t="s">
-        <v>1224</v>
+        <v>1220</v>
       </c>
       <c r="E115" s="197">
         <v>6.0059899999999999E-2</v>
       </c>
       <c r="F115" s="206" t="s">
-        <v>1178</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="15.75" thickBot="1">
@@ -16951,19 +16963,19 @@
         <v>49</v>
       </c>
       <c r="B116" s="215" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
       <c r="C116" s="20" t="s">
-        <v>1226</v>
+        <v>1222</v>
       </c>
       <c r="D116" s="204" t="s">
-        <v>1227</v>
+        <v>1223</v>
       </c>
       <c r="E116" s="203">
         <v>16.417300000000001</v>
       </c>
       <c r="F116" s="207" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="117" spans="1:9">
@@ -17023,12 +17035,12 @@
       <c r="A128" s="212"/>
       <c r="E128" s="14"/>
       <c r="I128" s="8" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="129" spans="1:17" ht="15.75" thickBot="1">
       <c r="A129" s="8" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="130" spans="1:17">
@@ -17036,13 +17048,13 @@
         <v>70</v>
       </c>
       <c r="B130" s="213" t="s">
-        <v>1229</v>
+        <v>1225</v>
       </c>
       <c r="C130" s="135" t="s">
-        <v>1229</v>
+        <v>1225</v>
       </c>
       <c r="D130" s="195" t="s">
-        <v>1230</v>
+        <v>1226</v>
       </c>
       <c r="E130" s="194">
         <v>3</v>
@@ -17054,13 +17066,13 @@
         <v>71</v>
       </c>
       <c r="B131" s="209" t="s">
-        <v>1231</v>
+        <v>1227</v>
       </c>
       <c r="C131" t="s">
-        <v>1231</v>
+        <v>1227</v>
       </c>
       <c r="D131" s="198" t="s">
-        <v>1232</v>
+        <v>1228</v>
       </c>
       <c r="E131" s="14">
         <v>6</v>
@@ -17072,13 +17084,13 @@
         <v>81</v>
       </c>
       <c r="B132" s="209" t="s">
-        <v>1233</v>
+        <v>1229</v>
       </c>
       <c r="C132" t="s">
-        <v>1233</v>
+        <v>1229</v>
       </c>
       <c r="D132" s="198" t="s">
-        <v>1234</v>
+        <v>1230</v>
       </c>
       <c r="E132" s="14">
         <v>500000</v>
@@ -17092,13 +17104,13 @@
         <v>74</v>
       </c>
       <c r="B133" s="209" t="s">
-        <v>1235</v>
+        <v>1231</v>
       </c>
       <c r="C133" t="s">
-        <v>1235</v>
+        <v>1231</v>
       </c>
       <c r="D133" s="198" t="s">
-        <v>1236</v>
+        <v>1232</v>
       </c>
       <c r="E133" s="14">
         <v>-3557.3522200000002</v>
@@ -17112,13 +17124,13 @@
         <v>80</v>
       </c>
       <c r="B134" s="215" t="s">
-        <v>1237</v>
+        <v>1233</v>
       </c>
       <c r="C134" s="20" t="s">
-        <v>1237</v>
+        <v>1233</v>
       </c>
       <c r="D134" s="204" t="s">
-        <v>1238</v>
+        <v>1234</v>
       </c>
       <c r="E134" s="202">
         <v>323.14999999999998</v>
@@ -17137,13 +17149,13 @@
     </row>
     <row r="138" spans="1:17" ht="15.75">
       <c r="A138" s="9" t="s">
-        <v>1249</v>
+        <v>1245</v>
       </c>
       <c r="I138" s="33"/>
     </row>
     <row r="139" spans="1:17" ht="15.75" thickBot="1">
       <c r="A139" s="8" t="s">
-        <v>1250</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="140" spans="1:17">
@@ -17151,13 +17163,13 @@
         <v>37</v>
       </c>
       <c r="B140" s="249" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
       <c r="C140" s="316" t="s">
         <v>191</v>
       </c>
       <c r="Q140" s="8" t="s">
-        <v>1304</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="141" spans="1:17" ht="15.75" thickBot="1">
@@ -17170,7 +17182,7 @@
     </row>
     <row r="142" spans="1:17">
       <c r="A142" s="318" t="s">
-        <v>1252</v>
+        <v>1248</v>
       </c>
       <c r="B142" s="225" t="s">
         <v>877</v>
@@ -17181,7 +17193,7 @@
     <row r="143" spans="1:17">
       <c r="A143" s="319"/>
       <c r="B143" s="226" t="s">
-        <v>1253</v>
+        <v>1249</v>
       </c>
       <c r="C143" s="198"/>
     </row>
@@ -17195,13 +17207,13 @@
     <row r="145" spans="1:3">
       <c r="A145" s="319"/>
       <c r="B145" s="230" t="s">
-        <v>1254</v>
+        <v>1250</v>
       </c>
       <c r="C145" s="198"/>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="319" t="s">
-        <v>1255</v>
+        <v>1251</v>
       </c>
       <c r="B146" s="226" t="s">
         <v>877</v>
@@ -17211,7 +17223,7 @@
     <row r="147" spans="1:3">
       <c r="A147" s="319"/>
       <c r="B147" s="226" t="s">
-        <v>1253</v>
+        <v>1249</v>
       </c>
       <c r="C147" s="198"/>
     </row>
@@ -17225,13 +17237,13 @@
     <row r="149" spans="1:3">
       <c r="A149" s="319"/>
       <c r="B149" s="226" t="s">
-        <v>1254</v>
+        <v>1250</v>
       </c>
       <c r="C149" s="198"/>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="197" t="s">
-        <v>1256</v>
+        <v>1252</v>
       </c>
       <c r="B150" s="226" t="b">
         <v>1</v>
@@ -17240,7 +17252,7 @@
     </row>
     <row r="151" spans="1:3">
       <c r="A151" s="197" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
       <c r="B151" s="226" t="b">
         <v>0</v>
@@ -17249,7 +17261,7 @@
     </row>
     <row r="152" spans="1:3">
       <c r="A152" s="319" t="s">
-        <v>1258</v>
+        <v>1254</v>
       </c>
       <c r="B152" s="226">
         <v>0.86609800000000003</v>
@@ -17279,7 +17291,7 @@
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="209" t="s">
-        <v>1283</v>
+        <v>1279</v>
       </c>
       <c r="B156" s="226">
         <v>100</v>
@@ -17290,35 +17302,35 @@
     </row>
     <row r="157" spans="1:3" ht="15.75" thickBot="1">
       <c r="A157" s="215" t="s">
-        <v>1284</v>
+        <v>1280</v>
       </c>
       <c r="B157" s="228">
         <v>5.7012200000000002</v>
       </c>
       <c r="C157" s="204" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="15.75" thickBot="1">
       <c r="A160" s="8" t="s">
-        <v>1305</v>
+        <v>1301</v>
       </c>
       <c r="B160" s="33"/>
     </row>
     <row r="161" spans="1:9">
       <c r="A161" s="213" t="s">
-        <v>1270</v>
+        <v>1266</v>
       </c>
       <c r="B161" s="213">
         <v>932.63499999999999</v>
       </c>
       <c r="C161" s="195" t="s">
-        <v>1161</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="162" spans="1:9">
       <c r="A162" s="209" t="s">
-        <v>1271</v>
+        <v>1267</v>
       </c>
       <c r="B162" s="209">
         <v>62640.6</v>
@@ -17329,40 +17341,40 @@
     </row>
     <row r="163" spans="1:9">
       <c r="A163" s="209" t="s">
-        <v>1272</v>
+        <v>1268</v>
       </c>
       <c r="B163" s="209">
         <v>51.753259399999997</v>
       </c>
       <c r="C163" s="198" t="s">
-        <v>1273</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="164" spans="1:9">
       <c r="A164" s="209" t="s">
-        <v>1274</v>
+        <v>1270</v>
       </c>
       <c r="B164" s="209">
         <v>-276652143</v>
       </c>
       <c r="C164" s="198" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="165" spans="1:9">
       <c r="A165" s="209" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="B165" s="209">
         <v>965.56</v>
       </c>
       <c r="C165" s="198" t="s">
-        <v>1303</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="166" spans="1:9">
       <c r="A166" s="209" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="B166" s="209">
         <v>18.020800000000001</v>
@@ -17371,18 +17383,18 @@
     </row>
     <row r="167" spans="1:9">
       <c r="A167" s="209" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
       <c r="B167" s="209">
         <v>5.5309200000000003E-2</v>
       </c>
       <c r="C167" s="198" t="s">
-        <v>1178</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="168" spans="1:9">
       <c r="A168" s="209" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
       <c r="B168" s="209">
         <v>386.01299999999998</v>
@@ -17393,18 +17405,18 @@
     </row>
     <row r="169" spans="1:9">
       <c r="A169" s="209" t="s">
-        <v>1280</v>
+        <v>1276</v>
       </c>
       <c r="B169" s="209">
         <v>2.41394E-4</v>
       </c>
       <c r="C169" s="198" t="s">
-        <v>1181</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="170" spans="1:9">
       <c r="A170" s="209" t="s">
-        <v>1281</v>
+        <v>1277</v>
       </c>
       <c r="B170" s="209">
         <v>180000</v>
@@ -17415,7 +17427,7 @@
     </row>
     <row r="171" spans="1:9">
       <c r="A171" s="209" t="s">
-        <v>1282</v>
+        <v>1278</v>
       </c>
       <c r="B171" s="209">
         <v>386.01299999999998</v>
@@ -17426,7 +17438,7 @@
     </row>
     <row r="172" spans="1:9">
       <c r="A172" s="209" t="s">
-        <v>1287</v>
+        <v>1283</v>
       </c>
       <c r="B172" s="209">
         <v>59202.400000000001</v>
@@ -17440,40 +17452,40 @@
     </row>
     <row r="173" spans="1:9">
       <c r="A173" s="209" t="s">
-        <v>1288</v>
+        <v>1284</v>
       </c>
       <c r="B173" s="209">
         <v>1.80208E-2</v>
       </c>
       <c r="C173" s="198" t="s">
-        <v>1180</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="174" spans="1:9">
       <c r="A174" s="209" t="s">
-        <v>1289</v>
+        <v>1285</v>
       </c>
       <c r="B174" s="209">
         <v>-212266540</v>
       </c>
       <c r="C174" s="198" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="175" spans="1:9">
       <c r="A175" s="209" t="s">
-        <v>1291</v>
+        <v>1287</v>
       </c>
       <c r="B175" s="209">
         <v>0.90935999999999995</v>
       </c>
       <c r="C175" s="198" t="s">
-        <v>1059</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="176" spans="1:9">
       <c r="A176" s="209" t="s">
-        <v>1292</v>
+        <v>1288</v>
       </c>
       <c r="B176" s="209">
         <v>18.02</v>
@@ -17482,7 +17494,7 @@
     </row>
     <row r="177" spans="1:9">
       <c r="A177" s="209" t="s">
-        <v>1293</v>
+        <v>1289</v>
       </c>
       <c r="B177" s="209">
         <v>390.39800000000002</v>
@@ -17493,24 +17505,24 @@
     </row>
     <row r="178" spans="1:9">
       <c r="A178" s="209" t="s">
-        <v>1294</v>
+        <v>1290</v>
       </c>
       <c r="B178" s="224">
         <v>1.3240299999999999E-5</v>
       </c>
       <c r="C178" s="198" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="179" spans="1:9" ht="15.75" thickBot="1">
       <c r="A179" s="229" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c r="B179" s="215">
         <v>60660.7</v>
       </c>
       <c r="C179" s="204" t="s">
-        <v>1179</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="180" spans="1:9">
@@ -17531,19 +17543,19 @@
     </row>
     <row r="183" spans="1:9">
       <c r="A183" s="213" t="s">
-        <v>1265</v>
+        <v>1261</v>
       </c>
       <c r="B183" s="213">
         <v>0.24</v>
       </c>
       <c r="C183" s="195" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
       <c r="F183" s="8"/>
     </row>
     <row r="184" spans="1:9">
       <c r="A184" s="209" t="s">
-        <v>1266</v>
+        <v>1262</v>
       </c>
       <c r="B184" s="209">
         <v>45.359200000000001</v>
@@ -17552,18 +17564,18 @@
         <v>480</v>
       </c>
       <c r="I184" s="8" t="s">
-        <v>1260</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="15.75" thickBot="1">
       <c r="A185" s="215" t="s">
-        <v>1267</v>
+        <v>1263</v>
       </c>
       <c r="B185" s="215">
         <v>2.5177999999999998</v>
       </c>
       <c r="C185" s="204" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="186" spans="1:9">
@@ -17576,13 +17588,13 @@
     </row>
     <row r="188" spans="1:9" ht="15.75" thickBot="1">
       <c r="A188" s="8" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
       <c r="B188" s="33"/>
     </row>
     <row r="189" spans="1:9">
       <c r="A189" s="213" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
       <c r="B189" s="213">
         <v>62898.329010000001</v>
@@ -17594,7 +17606,7 @@
     </row>
     <row r="190" spans="1:9">
       <c r="A190" s="209" t="s">
-        <v>1261</v>
+        <v>1257</v>
       </c>
       <c r="B190" s="209">
         <v>63186.050999999999</v>
@@ -17605,31 +17617,31 @@
     </row>
     <row r="191" spans="1:9">
       <c r="A191" s="209" t="s">
-        <v>1262</v>
+        <v>1258</v>
       </c>
       <c r="B191" s="209">
         <v>3491.4</v>
       </c>
       <c r="C191" s="198" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
       <c r="G191" s="33"/>
       <c r="H191" s="33"/>
     </row>
     <row r="192" spans="1:9">
       <c r="A192" s="209" t="s">
-        <v>1264</v>
+        <v>1260</v>
       </c>
       <c r="B192" s="209">
         <v>3507.52</v>
       </c>
       <c r="C192" s="198" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="193" spans="1:16">
       <c r="A193" s="209" t="s">
-        <v>1268</v>
+        <v>1264</v>
       </c>
       <c r="B193" s="209">
         <v>45.359200000000001</v>
@@ -17640,18 +17652,18 @@
     </row>
     <row r="194" spans="1:16">
       <c r="A194" s="209" t="s">
-        <v>1269</v>
+        <v>1265</v>
       </c>
       <c r="B194" s="209">
         <v>2.5177999999999998</v>
       </c>
       <c r="C194" s="198" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="195" spans="1:16">
       <c r="A195" s="209" t="s">
-        <v>1285</v>
+        <v>1281</v>
       </c>
       <c r="B195" s="209">
         <v>59800</v>
@@ -17662,24 +17674,24 @@
     </row>
     <row r="196" spans="1:16" ht="15.75" thickBot="1">
       <c r="A196" s="215" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="B196" s="215">
         <v>3319.56</v>
       </c>
       <c r="C196" s="204" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="203" spans="1:16" ht="15.75" thickBot="1">
       <c r="A203" s="8" t="s">
-        <v>1311</v>
+        <v>1307</v>
       </c>
       <c r="I203" s="8" t="s">
-        <v>1311</v>
+        <v>1307</v>
       </c>
       <c r="P203" s="8" t="s">
-        <v>1312</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="204" spans="1:16">
@@ -17690,13 +17702,13 @@
         <v>37</v>
       </c>
       <c r="C204" s="249" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="D204" s="249" t="s">
-        <v>1031</v>
+        <v>1027</v>
       </c>
       <c r="E204" s="249" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
       <c r="F204" s="249" t="s">
         <v>191</v>
@@ -17719,13 +17731,13 @@
         <v>60</v>
       </c>
       <c r="B206" s="213" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
       <c r="C206" s="135" t="s">
-        <v>1239</v>
+        <v>1235</v>
       </c>
       <c r="D206" s="135" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
       <c r="E206" s="216">
         <v>-38920792</v>
@@ -17741,10 +17753,10 @@
         <v>82</v>
       </c>
       <c r="B207" s="209" t="s">
-        <v>1240</v>
+        <v>1236</v>
       </c>
       <c r="C207" t="s">
-        <v>1241</v>
+        <v>1237</v>
       </c>
       <c r="E207" s="197"/>
       <c r="F207" s="206"/>
@@ -17756,10 +17768,10 @@
         <v>83</v>
       </c>
       <c r="B208" s="209" t="s">
-        <v>1242</v>
+        <v>1238</v>
       </c>
       <c r="C208" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="E208" s="197"/>
       <c r="F208" s="206"/>
@@ -17771,10 +17783,10 @@
         <v>84</v>
       </c>
       <c r="B209" s="209" t="s">
-        <v>1244</v>
+        <v>1240</v>
       </c>
       <c r="C209" t="s">
-        <v>1245</v>
+        <v>1241</v>
       </c>
       <c r="E209" s="197"/>
       <c r="F209" s="206"/>
@@ -17789,7 +17801,7 @@
         <v>85</v>
       </c>
       <c r="C210" s="20" t="s">
-        <v>1246</v>
+        <v>1242</v>
       </c>
       <c r="D210" s="20"/>
       <c r="E210" s="203"/>
@@ -17797,10 +17809,10 @@
       <c r="G210" s="14"/>
       <c r="H210" s="14"/>
       <c r="I210" s="8" t="s">
-        <v>1313</v>
+        <v>1309</v>
       </c>
       <c r="P210" s="8" t="s">
-        <v>1316</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="211" spans="1:16">
@@ -17812,7 +17824,7 @@
     </row>
     <row r="212" spans="1:16">
       <c r="A212" s="8" t="s">
-        <v>1314</v>
+        <v>1310</v>
       </c>
       <c r="E212" s="14"/>
       <c r="F212" s="14"/>
@@ -17940,7 +17952,7 @@
     </row>
     <row r="230" spans="1:8" ht="15.75" thickBot="1">
       <c r="A230" s="8" t="s">
-        <v>1312</v>
+        <v>1308</v>
       </c>
       <c r="B230" s="8"/>
       <c r="G230" s="14"/>
@@ -17954,13 +17966,13 @@
         <v>37</v>
       </c>
       <c r="C231" s="249" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="D231" s="249" t="s">
-        <v>1031</v>
+        <v>1027</v>
       </c>
       <c r="E231" s="249" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
       <c r="F231" s="249" t="s">
         <v>191</v>
@@ -17981,7 +17993,7 @@
         <v>61</v>
       </c>
       <c r="B233" s="213" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
       <c r="C233" s="135" t="s">
         <v>192</v>
@@ -17999,10 +18011,10 @@
         <v>86</v>
       </c>
       <c r="B234" s="209" t="s">
-        <v>1240</v>
+        <v>1236</v>
       </c>
       <c r="C234" t="s">
-        <v>1237</v>
+        <v>1233</v>
       </c>
       <c r="E234" s="209"/>
       <c r="F234" s="198"/>
@@ -18012,10 +18024,10 @@
         <v>87</v>
       </c>
       <c r="B235" s="209" t="s">
-        <v>1242</v>
+        <v>1238</v>
       </c>
       <c r="C235" t="s">
-        <v>1233</v>
+        <v>1229</v>
       </c>
       <c r="E235" s="209"/>
       <c r="F235" s="198"/>
@@ -18025,10 +18037,10 @@
         <v>88</v>
       </c>
       <c r="B236" s="209" t="s">
-        <v>1244</v>
+        <v>1240</v>
       </c>
       <c r="C236" t="s">
-        <v>1247</v>
+        <v>1243</v>
       </c>
       <c r="E236" s="209"/>
       <c r="F236" s="198"/>
@@ -18041,7 +18053,7 @@
         <v>85</v>
       </c>
       <c r="C237" s="20" t="s">
-        <v>1248</v>
+        <v>1244</v>
       </c>
       <c r="D237" s="20"/>
       <c r="E237" s="215"/>
@@ -18049,7 +18061,7 @@
     </row>
     <row r="239" spans="1:8">
       <c r="A239" s="8" t="s">
-        <v>1315</v>
+        <v>1311</v>
       </c>
     </row>
   </sheetData>
@@ -18286,7 +18298,7 @@
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1">
       <c r="A33" t="s">
-        <v>1324</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="16.5" thickBot="1">
@@ -18307,7 +18319,7 @@
         <v>37</v>
       </c>
       <c r="B36" s="240" t="s">
-        <v>1028</v>
+        <v>1024</v>
       </c>
       <c r="C36" s="240" t="s">
         <v>75</v>
@@ -19313,7 +19325,7 @@
         <v>96</v>
       </c>
       <c r="F18" s="245" t="s">
-        <v>1027</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
@@ -20247,7 +20259,7 @@
     </row>
     <row r="7" spans="1:44" ht="18" thickBot="1">
       <c r="A7" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="I7" s="89" t="s">
         <v>550</v>
@@ -20952,7 +20964,7 @@
         <v>37</v>
       </c>
       <c r="C64" s="245" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="D64" s="245" t="s">
         <v>504</v>
@@ -21540,7 +21552,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -21608,7 +21620,7 @@
         <v>73</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>1319</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -21627,7 +21639,7 @@
     </row>
     <row r="21" spans="1:7" ht="15.75">
       <c r="A21" s="270" t="s">
-        <v>1026</v>
+        <v>1022</v>
       </c>
       <c r="B21" s="271"/>
       <c r="C21" s="271"/>
@@ -23175,7 +23187,7 @@
       <c r="D138" s="70"/>
       <c r="E138" s="72"/>
       <c r="G138" s="8" t="s">
-        <v>1320</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="45" hidden="1" customHeight="1">
@@ -23318,7 +23330,7 @@
     </row>
     <row r="151" spans="1:5" ht="16.5" thickBot="1">
       <c r="A151" s="265" t="s">
-        <v>1025</v>
+        <v>1021</v>
       </c>
       <c r="B151" s="266"/>
       <c r="C151" s="266"/>
@@ -26470,7 +26482,7 @@
         <v>96</v>
       </c>
       <c r="E19" s="286" t="s">
-        <v>1321</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1">

</xml_diff>